<commit_message>
BIS-1803: Add CLI options for multiple TTL files
</commit_message>
<xml_diff>
--- a/lib-rdf/src/test/resources/expected_output.xlsx
+++ b/lib-rdf/src/test/resources/expected_output.xlsx
@@ -391,12 +391,12 @@
     <t>Code-SNOMED-CT-308829001</t>
   </si>
   <si>
+    <t>hasIdentifier</t>
+  </si>
+  <si>
     <t>hasName</t>
   </si>
   <si>
-    <t>hasIdentifier</t>
-  </si>
-  <si>
     <t>hasCodingSystemAndVersion</t>
   </si>
   <si>
@@ -406,13 +406,13 @@
     <t>CHE-229_707_417-Code-7a024204-f7c1-4d87-8da5-e709d4713d60</t>
   </si>
   <si>
+    <t>/DEFAULT/SPHN/adipisicing adipisicing adipisicing reprehenderit</t>
+  </si>
+  <si>
+    <t>/DEFAULT/SPHN/ID-593824-iWg</t>
+  </si>
+  <si>
     <t>/DEFAULT/SPHN/odit reprehenderit Lorem accusantium</t>
-  </si>
-  <si>
-    <t>/DEFAULT/SPHN/ID-593824-iWg</t>
-  </si>
-  <si>
-    <t>/DEFAULT/SPHN/adipisicing adipisicing adipisicing reprehenderit</t>
   </si>
   <si>
     <t>hasCode</t>
@@ -2019,13 +2019,13 @@
         <v>124</v>
       </c>
       <c r="J21" t="s">
+        <v>126</v>
+      </c>
+      <c r="K21" t="s">
+        <v>127</v>
+      </c>
+      <c r="L21" t="s">
         <v>125</v>
-      </c>
-      <c r="K21" t="s">
-        <v>126</v>
-      </c>
-      <c r="L21" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="22"/>

</xml_diff>